<commit_message>
just need serial numbers
</commit_message>
<xml_diff>
--- a/tagsheet_to_tidbits2025/data/Sander's PIT CODES.xlsx
+++ b/tagsheet_to_tidbits2025/data/Sander's PIT CODES.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umainesystem-my.sharepoint.com/personal/sander_elliott_maine_edu/Documents/Desktop/Github/Sturgeon_TidBits/tagsheet_to_tidbits2025/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f03cf4e0d6e7cfb9/Desktop/Code/Sturgeon_TidBits/tagsheet_to_tidbits2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{87E30D02-C812-421C-A0AA-2F4032EB8D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0DE24BD-F43B-40F1-BFF1-7D219A7994F7}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{87E30D02-C812-421C-A0AA-2F4032EB8D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C72B015-15B0-438A-B96A-E871B20D540E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip" sheetId="7" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="Trip(1)" sheetId="2" r:id="rId3"/>
-    <sheet name="Trip (2)" sheetId="8" r:id="rId4"/>
-    <sheet name="Trip (3)" sheetId="9" r:id="rId5"/>
-    <sheet name="Trip (4)" sheetId="11" r:id="rId6"/>
-    <sheet name="Trip (5)" sheetId="12" r:id="rId7"/>
+    <sheet name="Sheet1 (2)" sheetId="13" r:id="rId3"/>
+    <sheet name="Trip(1)" sheetId="2" r:id="rId4"/>
+    <sheet name="Trip (2)" sheetId="8" r:id="rId5"/>
+    <sheet name="Trip (3)" sheetId="9" r:id="rId6"/>
+    <sheet name="Trip (4)" sheetId="11" r:id="rId7"/>
+    <sheet name="Trip (5)" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="214">
   <si>
     <t>3DD.003E185F8C</t>
   </si>
@@ -543,13 +544,151 @@
   </si>
   <si>
     <t>NO RIGHT PEC</t>
+  </si>
+  <si>
+    <t>1645258</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>MAINE DEPT OF MARINE RESOURCES</t>
+  </si>
+  <si>
+    <t>Joseph Zydlewski</t>
+  </si>
+  <si>
+    <t>V16-4x-BLU-1</t>
+  </si>
+  <si>
+    <t>1645259</t>
+  </si>
+  <si>
+    <t>1645260</t>
+  </si>
+  <si>
+    <t>1645261</t>
+  </si>
+  <si>
+    <t>1645262</t>
+  </si>
+  <si>
+    <t>1645263</t>
+  </si>
+  <si>
+    <t>1645264</t>
+  </si>
+  <si>
+    <t>1645265</t>
+  </si>
+  <si>
+    <t>1645266</t>
+  </si>
+  <si>
+    <t>1645267</t>
+  </si>
+  <si>
+    <t>1645268</t>
+  </si>
+  <si>
+    <t>1645269</t>
+  </si>
+  <si>
+    <t>1645270</t>
+  </si>
+  <si>
+    <t>1645271</t>
+  </si>
+  <si>
+    <t>1645272</t>
+  </si>
+  <si>
+    <t>1645273</t>
+  </si>
+  <si>
+    <t>1645274</t>
+  </si>
+  <si>
+    <t>1645275</t>
+  </si>
+  <si>
+    <t>1645276</t>
+  </si>
+  <si>
+    <t>1645277</t>
+  </si>
+  <si>
+    <t>1645278</t>
+  </si>
+  <si>
+    <t>1645279</t>
+  </si>
+  <si>
+    <t>1645280</t>
+  </si>
+  <si>
+    <t>1645281</t>
+  </si>
+  <si>
+    <t>1645282</t>
+  </si>
+  <si>
+    <t>1645283</t>
+  </si>
+  <si>
+    <t>1645284</t>
+  </si>
+  <si>
+    <t>1645285</t>
+  </si>
+  <si>
+    <t>1645286</t>
+  </si>
+  <si>
+    <t>1645287</t>
+  </si>
+  <si>
+    <t>1645288</t>
+  </si>
+  <si>
+    <t>1645289</t>
+  </si>
+  <si>
+    <t>1645290</t>
+  </si>
+  <si>
+    <t>1645291</t>
+  </si>
+  <si>
+    <t>1645292</t>
+  </si>
+  <si>
+    <t>1645293</t>
+  </si>
+  <si>
+    <t>1645294</t>
+  </si>
+  <si>
+    <t>1645295</t>
+  </si>
+  <si>
+    <t>1645296</t>
+  </si>
+  <si>
+    <t>1645297</t>
+  </si>
+  <si>
+    <t>1645298</t>
+  </si>
+  <si>
+    <t>1645299</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -689,6 +828,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1078,7 +1222,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1121,8 +1265,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -1150,8 +1295,10 @@
     <xf numFmtId="0" fontId="17" fillId="13" borderId="11" xfId="22" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1189,13 +1336,24 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="42" xr:uid="{8D2619A1-7999-4244-81BC-02B86FBC88EF}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1606,29 +1764,29 @@
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" customWidth="1"/>
+    <col min="11" max="11" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7265625" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" customWidth="1"/>
     <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>88</v>
       </c>
@@ -1699,7 +1857,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
       <c r="H2" s="5"/>
@@ -1726,7 +1884,7 @@
       </c>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F3" s="2"/>
       <c r="H3" s="8"/>
       <c r="I3" s="2"/>
@@ -1744,7 +1902,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F4" s="2"/>
       <c r="H4" s="8"/>
       <c r="I4" s="2"/>
@@ -1762,7 +1920,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F5" s="2"/>
       <c r="H5" s="8"/>
       <c r="I5" s="2"/>
@@ -1780,7 +1938,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F6" s="2"/>
       <c r="H6" s="8"/>
       <c r="I6" s="2"/>
@@ -1798,7 +1956,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F7" s="2"/>
       <c r="H7" s="8"/>
       <c r="I7" s="2"/>
@@ -1816,7 +1974,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F8" s="2"/>
       <c r="H8" s="9"/>
       <c r="I8" s="2"/>
@@ -1834,7 +1992,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -1852,7 +2010,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -1870,7 +2028,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1888,7 +2046,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1902,7 +2060,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -1916,7 +2074,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -1930,7 +2088,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -1944,7 +2102,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -1958,7 +2116,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1972,7 +2130,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1986,7 +2144,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -2000,7 +2158,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -2014,7 +2172,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -2028,7 +2186,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -2042,7 +2200,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -2056,7 +2214,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -2070,7 +2228,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -2084,7 +2242,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -2098,7 +2256,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -2112,7 +2270,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -2126,7 +2284,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -2140,7 +2298,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -2154,7 +2312,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -2168,7 +2326,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -2182,7 +2340,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -2196,7 +2354,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -2210,7 +2368,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -2220,7 +2378,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -2230,25 +2388,25 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="Q2:Q100">
-    <cfRule type="expression" dxfId="12" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="1" stopIfTrue="1">
       <formula>AND($Q2&lt;&gt;$B2, $Q2&lt;&gt;"UKN", $Q2&lt;&gt;"", $B2&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$Q2="UKN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="3" stopIfTrue="1">
       <formula>AND($Q2=$B2, $Q2&lt;&gt;"", $B2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2261,16 +2419,16 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -2287,7 +2445,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2305,7 +2463,7 @@
         <v>201133</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2323,7 +2481,7 @@
         <v>201127</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2341,7 +2499,7 @@
         <v>201134</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2359,7 +2517,7 @@
         <v>201128</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2377,7 +2535,7 @@
         <v>201129</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2395,7 +2553,7 @@
         <v>201131</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2413,7 +2571,7 @@
         <v>201130</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2431,7 +2589,7 @@
         <v>201132</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2449,7 +2607,7 @@
         <v>201212</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2467,7 +2625,7 @@
         <v>201215</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2485,7 +2643,7 @@
         <v>201213</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2503,7 +2661,7 @@
         <v>201214</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2521,7 +2679,7 @@
         <v>201216</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2539,7 +2697,7 @@
         <v>201217</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2557,7 +2715,7 @@
         <v>201218</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2575,7 +2733,7 @@
         <v>201219</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2593,7 +2751,7 @@
         <v>201220</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2611,7 +2769,7 @@
         <v>201223</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2629,7 +2787,7 @@
         <v>201222</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2647,7 +2805,7 @@
         <v>201221</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2665,7 +2823,7 @@
         <v>201224</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2683,7 +2841,7 @@
         <v>201225</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2701,7 +2859,7 @@
         <v>201226</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2719,7 +2877,7 @@
         <v>201227</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2737,7 +2895,7 @@
         <v>201228</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2755,7 +2913,7 @@
         <v>201229</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2773,7 +2931,7 @@
         <v>201232</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2791,7 +2949,7 @@
         <v>201231</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2809,7 +2967,7 @@
         <v>201230</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2827,7 +2985,7 @@
         <v>201235</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2845,7 +3003,7 @@
         <v>201234</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2863,7 +3021,7 @@
         <v>201233</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2881,7 +3039,7 @@
         <v>201238</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2899,7 +3057,7 @@
         <v>201237</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2917,7 +3075,7 @@
         <v>201236</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2935,7 +3093,7 @@
         <v>201239</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2953,7 +3111,7 @@
         <v>201240</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2971,7 +3129,7 @@
         <v>201241</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2989,7 +3147,7 @@
         <v>201244</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3007,7 +3165,7 @@
         <v>201243</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3025,7 +3183,7 @@
         <v>201242</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3043,7 +3201,7 @@
         <v>201247</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3061,7 +3219,7 @@
         <v>201246</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3079,7 +3237,7 @@
         <v>201245</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3097,7 +3255,7 @@
         <v>201252</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3115,7 +3273,7 @@
         <v>201249</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3133,7 +3291,7 @@
         <v>201253</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3151,7 +3309,7 @@
         <v>201250</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3169,7 +3327,7 @@
         <v>201248</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3187,7 +3345,7 @@
         <v>201251</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3195,7 +3353,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3203,7 +3361,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3211,7 +3369,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3219,7 +3377,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3227,7 +3385,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3235,7 +3393,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3243,7 +3401,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3251,7 +3409,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3259,7 +3417,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3271,7 +3429,7 @@
   <sheetProtection algorithmName="SHA-512" hashValue="GLBxjVtZqvzkQTPGUZuo+WHi4zuX2+iRK7ponll4YJu7jFzCXRgL29u+SxlJRXoxg9VxoqC0XidWHTkVsfdCng==" saltValue="otX8nHZYZ6RQ5YCUGUc8Og==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="F2:F51">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3279,6 +3437,1782 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0019F054-F7CA-421F-8EA8-E60A6BBFF39A}">
+  <dimension ref="A1:M61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <f>VALUE(RIGHT(E2,6))</f>
+        <v>201133</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F51" si="0">VALUE(RIGHT(E3,6))</f>
+        <v>201127</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>201134</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>201128</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>201129</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>201131</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>201130</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>201132</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>201212</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>201215</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L11" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>201213</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>201214</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M13" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>201216</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>201217</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>201218</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L16" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>201219</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L17" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>201220</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="I18" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L18" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>201223</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>201222</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L20" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>201221</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>201224</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L22" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>201225</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>201226</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L24" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>201227</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J25" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L25" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>201228</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="I26" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J26" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L26" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M26" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>201229</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J27" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L27" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>201232</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>201231</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L29" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M29" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>201230</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J30" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L30" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M30" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>201235</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="I31" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L31" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M31" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32">
+        <v>31</v>
+      </c>
+      <c r="E32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>201234</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L32" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M32" s="15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+      <c r="E33" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>201233</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="I33" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L33" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M33" s="15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <v>33</v>
+      </c>
+      <c r="E34" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>201238</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L34" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M34" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35">
+        <v>34</v>
+      </c>
+      <c r="E35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>201237</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L35" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M35" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <v>35</v>
+      </c>
+      <c r="E36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>201236</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J36" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L36" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M36" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37">
+        <v>36</v>
+      </c>
+      <c r="E37" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>201239</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K37" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L37" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38">
+        <v>37</v>
+      </c>
+      <c r="E38" t="s">
+        <v>111</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>201240</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L38" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M38" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39">
+        <v>38</v>
+      </c>
+      <c r="E39" t="s">
+        <v>112</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>201241</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L39" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M39" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40">
+        <v>39</v>
+      </c>
+      <c r="E40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>201244</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J40" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L40" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M40" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41">
+        <v>40</v>
+      </c>
+      <c r="E41" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>201243</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="I41" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J41" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K41" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L41" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M41" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42">
+        <v>41</v>
+      </c>
+      <c r="E42" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>201242</v>
+      </c>
+      <c r="H42" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K42" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L42" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M42" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43">
+        <v>42</v>
+      </c>
+      <c r="E43" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>201247</v>
+      </c>
+      <c r="H43" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="K43" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="L43" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="M43" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44">
+        <v>43</v>
+      </c>
+      <c r="E44" t="s">
+        <v>117</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>201246</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45">
+        <v>44</v>
+      </c>
+      <c r="E45" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>201245</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>162</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>201252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47">
+        <v>46</v>
+      </c>
+      <c r="E47" t="s">
+        <v>157</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>201249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48">
+        <v>47</v>
+      </c>
+      <c r="E48" t="s">
+        <v>158</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>201253</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49">
+        <v>48</v>
+      </c>
+      <c r="E49" t="s">
+        <v>159</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>201250</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D50">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>160</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>201248</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51">
+        <v>50</v>
+      </c>
+      <c r="E51" t="s">
+        <v>161</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>201251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F2:F51">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FD9965-3A02-44AF-9BF4-86BFA009B4F7}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
@@ -3286,29 +5220,29 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" customWidth="1"/>
+    <col min="11" max="11" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" customWidth="1"/>
     <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>88</v>
       </c>
@@ -3379,7 +5313,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3448,7 +5382,7 @@
         <v>4899033</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3502,7 +5436,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3556,7 +5490,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3608,7 +5542,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3662,7 +5596,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3719,7 +5653,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3773,7 +5707,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3827,7 +5761,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3884,7 +5818,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3941,163 +5875,163 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:10" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
     </row>
   </sheetData>
@@ -4106,7 +6040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A83D4C17-C0AD-48BE-80DF-6BA497415298}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
@@ -4114,29 +6048,29 @@
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" customWidth="1"/>
+    <col min="11" max="11" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" customWidth="1"/>
     <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>88</v>
       </c>
@@ -4207,7 +6141,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>11</v>
       </c>
@@ -4276,7 +6210,7 @@
         <v>4902372</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>12</v>
       </c>
@@ -4330,7 +6264,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13</v>
       </c>
@@ -4384,7 +6318,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>14</v>
       </c>
@@ -4441,7 +6375,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>15</v>
       </c>
@@ -4498,7 +6432,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16</v>
       </c>
@@ -4555,7 +6489,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>17</v>
       </c>
@@ -4609,7 +6543,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>18</v>
       </c>
@@ -4663,7 +6597,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>19</v>
       </c>
@@ -4717,7 +6651,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>20</v>
       </c>
@@ -4771,7 +6705,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>21</v>
       </c>
@@ -4825,7 +6759,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>22</v>
       </c>
@@ -4879,7 +6813,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>23</v>
       </c>
@@ -4933,7 +6867,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>24</v>
       </c>
@@ -4984,7 +6918,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -4994,7 +6928,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -5004,7 +6938,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -5014,7 +6948,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -5024,7 +6958,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -5034,7 +6968,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -5044,7 +6978,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -5054,7 +6988,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -5064,7 +6998,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -5074,7 +7008,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -5084,7 +7018,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -5094,7 +7028,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -5104,7 +7038,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -5114,7 +7048,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -5124,7 +7058,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -5134,7 +7068,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -5144,7 +7078,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -5154,7 +7088,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -5164,7 +7098,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -5174,7 +7108,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -5184,7 +7118,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -5194,13 +7128,13 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
     </row>
   </sheetData>
@@ -5209,37 +7143,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{488E39B3-2C61-459C-8BA6-3DDB189E9E40}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" customWidth="1"/>
+    <col min="11" max="11" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7265625" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" customWidth="1"/>
     <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>88</v>
       </c>
@@ -5310,7 +7244,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>25</v>
       </c>
@@ -5381,7 +7315,7 @@
         <v>4948116</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>26</v>
       </c>
@@ -5432,7 +7366,7 @@
         <v>SNS</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>27</v>
       </c>
@@ -5483,7 +7417,7 @@
         <v>SNS</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>28</v>
       </c>
@@ -5534,7 +7468,7 @@
         <v>SNS</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>29</v>
       </c>
@@ -5585,7 +7519,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>30</v>
       </c>
@@ -5636,7 +7570,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>31</v>
       </c>
@@ -5690,7 +7624,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>32</v>
       </c>
@@ -5743,7 +7677,7 @@
         <v>UKN</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>33</v>
       </c>
@@ -5796,7 +7730,7 @@
         <v>UKN</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>34</v>
       </c>
@@ -5849,7 +7783,7 @@
         <v>SNS</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>35</v>
       </c>
@@ -5900,7 +7834,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>36</v>
       </c>
@@ -5951,7 +7885,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>37</v>
       </c>
@@ -6002,7 +7936,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>38</v>
       </c>
@@ -6056,7 +7990,7 @@
         <v>SNS</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>39</v>
       </c>
@@ -6107,7 +8041,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="17" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N17" t="str">
         <f>IF(C17="", "", _xlfn.XLOOKUP(C17, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6117,7 +8051,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N18" t="str">
         <f>IF(C18="", "", _xlfn.XLOOKUP(C18, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6127,7 +8061,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N19" t="str">
         <f>IF(C19="", "", _xlfn.XLOOKUP(C19, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6137,7 +8071,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N20" t="str">
         <f>IF(C20="", "", _xlfn.XLOOKUP(C20, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6147,7 +8081,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N21" t="str">
         <f>IF(C21="", "", _xlfn.XLOOKUP(C21, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6157,7 +8091,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N22" t="str">
         <f>IF(C22="", "", _xlfn.XLOOKUP(C22, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6167,7 +8101,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N23" t="str">
         <f>IF(C23="", "", _xlfn.XLOOKUP(C23, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6177,7 +8111,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N24" t="str">
         <f>IF(C24="", "", _xlfn.XLOOKUP(C24, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6187,7 +8121,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N25" t="str">
         <f>IF(C25="", "", _xlfn.XLOOKUP(C25, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6197,7 +8131,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N26" t="str">
         <f>IF(C26="", "", _xlfn.XLOOKUP(C26, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6207,7 +8141,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N27" t="str">
         <f>IF(C27="", "", _xlfn.XLOOKUP(C27, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6217,7 +8151,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N28" t="str">
         <f>IF(C28="", "", _xlfn.XLOOKUP(C28, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6227,7 +8161,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N29" t="str">
         <f>IF(C29="", "", _xlfn.XLOOKUP(C29, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6237,7 +8171,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N30" t="str">
         <f>IF(C30="", "", _xlfn.XLOOKUP(C30, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6247,7 +8181,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N31" t="str">
         <f>IF(C31="", "", _xlfn.XLOOKUP(C31, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6257,7 +8191,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N32" t="str">
         <f>IF(C32="", "", _xlfn.XLOOKUP(C32, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6267,7 +8201,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N33" t="str">
         <f>IF(C33="", "", _xlfn.XLOOKUP(C33, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6277,7 +8211,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N34" t="str">
         <f>IF(C34="", "", _xlfn.XLOOKUP(C34, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6287,13 +8221,13 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N35" t="str">
         <f>IF(C35="", "", _xlfn.XLOOKUP(C35, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="14:15" x14ac:dyDescent="0.35">
       <c r="N36" t="str">
         <f>IF(C36="", "", _xlfn.XLOOKUP(C36, Sheet1!A:A, Sheet1!B:B, ""))</f>
         <v/>
@@ -6301,13 +8235,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q2:Q36">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>$Q2="UKN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="2" stopIfTrue="1">
       <formula>AND($Q2=$B2, $Q2&lt;&gt;"", $B2&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
       <formula>AND($Q2&lt;&gt;$B2, $Q2&lt;&gt;"UKN", $Q2&lt;&gt;"", $B2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6315,7 +8249,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DEAEC3-E597-43CF-8A39-542D98AFB6F7}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
@@ -6323,29 +8257,29 @@
       <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" customWidth="1"/>
+    <col min="11" max="11" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7265625" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" customWidth="1"/>
     <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>88</v>
       </c>
@@ -6416,7 +8350,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>40</v>
       </c>
@@ -6485,7 +8419,7 @@
         <v>4948116</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>41</v>
       </c>
@@ -6536,7 +8470,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>42</v>
       </c>
@@ -6587,7 +8521,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>43</v>
       </c>
@@ -6635,7 +8569,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>44</v>
       </c>
@@ -6683,7 +8617,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>45</v>
       </c>
@@ -6734,7 +8668,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>46</v>
       </c>
@@ -6782,7 +8716,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>47</v>
       </c>
@@ -6830,7 +8764,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>48</v>
       </c>
@@ -6881,7 +8815,7 @@
         <v>AST</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>49</v>
       </c>
@@ -6932,7 +8866,7 @@
         <v>SNS</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>50</v>
       </c>
@@ -6983,7 +8917,7 @@
         <v>SNS</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>51</v>
       </c>
@@ -7036,7 +8970,7 @@
         <v>SNS</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -7050,7 +8984,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -7064,7 +8998,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -7078,7 +9012,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -7092,7 +9026,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -7106,7 +9040,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -7120,7 +9054,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -7134,7 +9068,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -7148,7 +9082,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -7162,7 +9096,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -7176,7 +9110,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -7190,7 +9124,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -7204,7 +9138,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -7218,7 +9152,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -7232,7 +9166,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -7246,7 +9180,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -7260,7 +9194,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -7274,7 +9208,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -7288,7 +9222,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -7302,7 +9236,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -7316,7 +9250,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -7330,7 +9264,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -7340,7 +9274,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -7350,25 +9284,25 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="Q2:Q100">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>AND($Q2&lt;&gt;$B2, $Q2&lt;&gt;"UKN", $Q2&lt;&gt;"", $B2&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$Q2="UKN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>AND($Q2=$B2, $Q2&lt;&gt;"", $B2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7376,7 +9310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7092AF79-999B-48C9-8AAD-B4913AEC6A18}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
@@ -7384,29 +9318,29 @@
       <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.54296875" customWidth="1"/>
+    <col min="10" max="10" width="7.7265625" customWidth="1"/>
+    <col min="11" max="11" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7265625" customWidth="1"/>
+    <col min="17" max="17" width="12.1796875" customWidth="1"/>
     <col min="18" max="18" width="4" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="13" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="12" t="s">
         <v>88</v>
       </c>
@@ -7477,7 +9411,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>52</v>
       </c>
@@ -7549,7 +9483,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>53</v>
       </c>
@@ -7605,7 +9539,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>54</v>
       </c>
@@ -7659,7 +9593,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>55</v>
       </c>
@@ -7713,7 +9647,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>56</v>
       </c>
@@ -7767,7 +9701,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>57</v>
       </c>
@@ -7818,7 +9752,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>58</v>
       </c>
@@ -7869,7 +9803,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>59</v>
       </c>
@@ -7920,7 +9854,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>60</v>
       </c>
@@ -7971,7 +9905,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>61</v>
       </c>
@@ -8022,7 +9956,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>62</v>
       </c>
@@ -8073,7 +10007,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>63</v>
       </c>
@@ -8126,7 +10060,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -8140,7 +10074,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -8154,7 +10088,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="F16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -8168,7 +10102,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -8182,7 +10116,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -8196,7 +10130,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -8210,7 +10144,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -8224,7 +10158,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -8238,7 +10172,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -8252,7 +10186,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -8266,7 +10200,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -8280,7 +10214,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -8294,7 +10228,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -8308,7 +10242,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -8322,7 +10256,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -8336,7 +10270,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -8350,7 +10284,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -8364,7 +10298,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -8378,7 +10312,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -8392,7 +10326,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -8406,7 +10340,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -8420,7 +10354,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -8430,7 +10364,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -8440,25 +10374,25 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="Q2:Q100">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>AND($Q2&lt;&gt;$B2, $Q2&lt;&gt;"UKN", $Q2&lt;&gt;"", $B2&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$Q2="UKN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>AND($Q2=$B2, $Q2&lt;&gt;"", $B2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Separating by event not tag
</commit_message>
<xml_diff>
--- a/tagsheet_to_tidbits2025/data/Sander's PIT CODES.xlsx
+++ b/tagsheet_to_tidbits2025/data/Sander's PIT CODES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umainesystem-my.sharepoint.com/personal/sander_elliott_maine_edu/Documents/Desktop/Github/Sturgeon_TidBits/tagsheet_to_tidbits2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{87E30D02-C812-421C-A0AA-2F4032EB8D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D613798-27E4-42F6-8F60-023531AB6DF7}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{87E30D02-C812-421C-A0AA-2F4032EB8D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAA3E067-F1CF-4C23-BA8A-A0A1D0F9DE7B}"/>
   <bookViews>
-    <workbookView xWindow="29070" yWindow="0" windowWidth="28530" windowHeight="15480" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28755" yWindow="285" windowWidth="28530" windowHeight="15480" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trip" sheetId="7" r:id="rId1"/>
@@ -1148,7 +1148,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -1176,7 +1176,6 @@
     <xf numFmtId="0" fontId="17" fillId="13" borderId="11" xfId="22" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1339,6 +1338,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3371,7 +3374,7 @@
         <f>VALUE(RIGHT(E2,6))</f>
         <v>201133</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2">
         <v>1645258</v>
       </c>
       <c r="I2" t="s">
@@ -3395,7 +3398,7 @@
         <f t="shared" ref="F3:F51" si="0">VALUE(RIGHT(E3,6))</f>
         <v>201127</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3">
         <v>1645259</v>
       </c>
       <c r="I3" t="s">
@@ -3428,7 +3431,7 @@
         <f t="shared" si="0"/>
         <v>201134</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4">
         <v>1645260</v>
       </c>
       <c r="I4" t="s">
@@ -3464,7 +3467,7 @@
         <f t="shared" si="0"/>
         <v>201128</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5">
         <v>1645261</v>
       </c>
       <c r="I5" t="s">
@@ -3500,7 +3503,7 @@
         <f t="shared" si="0"/>
         <v>201129</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6">
         <v>1645262</v>
       </c>
       <c r="I6" t="s">
@@ -3536,7 +3539,7 @@
         <f t="shared" si="0"/>
         <v>201131</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7">
         <v>1645263</v>
       </c>
       <c r="I7" t="s">
@@ -3572,7 +3575,7 @@
         <f t="shared" si="0"/>
         <v>201130</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8">
         <v>1645264</v>
       </c>
       <c r="I8" t="s">
@@ -3608,7 +3611,7 @@
         <f t="shared" si="0"/>
         <v>201132</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9">
         <v>1645265</v>
       </c>
       <c r="I9" t="s">
@@ -3644,7 +3647,7 @@
         <f t="shared" si="0"/>
         <v>201212</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10">
         <v>1645266</v>
       </c>
       <c r="I10" t="s">
@@ -3680,7 +3683,7 @@
         <f t="shared" si="0"/>
         <v>201215</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11">
         <v>1645267</v>
       </c>
       <c r="I11" t="s">
@@ -3716,7 +3719,7 @@
         <f t="shared" si="0"/>
         <v>201213</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12">
         <v>1645268</v>
       </c>
       <c r="I12" t="s">
@@ -3752,7 +3755,7 @@
         <f t="shared" si="0"/>
         <v>201214</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13">
         <v>1645269</v>
       </c>
       <c r="I13" t="s">
@@ -3788,7 +3791,7 @@
         <f t="shared" si="0"/>
         <v>201216</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14">
         <v>1645270</v>
       </c>
       <c r="I14" t="s">
@@ -3824,7 +3827,7 @@
         <f t="shared" si="0"/>
         <v>201217</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15">
         <v>1645271</v>
       </c>
       <c r="I15" t="s">
@@ -3860,7 +3863,7 @@
         <f t="shared" si="0"/>
         <v>201218</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16">
         <v>1645272</v>
       </c>
       <c r="I16" t="s">
@@ -3896,7 +3899,7 @@
         <f t="shared" si="0"/>
         <v>201219</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17">
         <v>1645273</v>
       </c>
       <c r="I17" t="s">
@@ -3932,7 +3935,7 @@
         <f t="shared" si="0"/>
         <v>201220</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18">
         <v>1645274</v>
       </c>
       <c r="I18" t="s">
@@ -3968,7 +3971,7 @@
         <f t="shared" si="0"/>
         <v>201223</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19">
         <v>1645275</v>
       </c>
       <c r="I19" t="s">
@@ -4004,7 +4007,7 @@
         <f t="shared" si="0"/>
         <v>201222</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20">
         <v>1645276</v>
       </c>
       <c r="I20" t="s">
@@ -4040,7 +4043,7 @@
         <f t="shared" si="0"/>
         <v>201221</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21">
         <v>1645277</v>
       </c>
       <c r="I21" t="s">
@@ -4076,7 +4079,7 @@
         <f t="shared" si="0"/>
         <v>201224</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22">
         <v>1645278</v>
       </c>
       <c r="I22" t="s">
@@ -4112,7 +4115,7 @@
         <f t="shared" si="0"/>
         <v>201225</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H23">
         <v>1645279</v>
       </c>
       <c r="I23" t="s">
@@ -4148,7 +4151,7 @@
         <f t="shared" si="0"/>
         <v>201226</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24">
         <v>1645280</v>
       </c>
       <c r="I24" t="s">
@@ -4184,7 +4187,7 @@
         <f t="shared" si="0"/>
         <v>201227</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25">
         <v>1645281</v>
       </c>
       <c r="I25" t="s">
@@ -4220,7 +4223,7 @@
         <f t="shared" si="0"/>
         <v>201228</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26">
         <v>1645282</v>
       </c>
       <c r="I26" t="s">
@@ -4256,7 +4259,7 @@
         <f t="shared" si="0"/>
         <v>201229</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27">
         <v>1645283</v>
       </c>
       <c r="I27" t="s">
@@ -4292,7 +4295,7 @@
         <f t="shared" si="0"/>
         <v>201232</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28">
         <v>1645284</v>
       </c>
       <c r="I28" t="s">
@@ -4328,7 +4331,7 @@
         <f t="shared" si="0"/>
         <v>201231</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29">
         <v>1645285</v>
       </c>
       <c r="I29" t="s">
@@ -4364,7 +4367,7 @@
         <f t="shared" si="0"/>
         <v>201230</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30">
         <v>1645286</v>
       </c>
       <c r="I30" t="s">
@@ -4400,7 +4403,7 @@
         <f t="shared" si="0"/>
         <v>201235</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31">
         <v>1645287</v>
       </c>
       <c r="I31" t="s">
@@ -4436,7 +4439,7 @@
         <f t="shared" si="0"/>
         <v>201234</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32">
         <v>1645288</v>
       </c>
       <c r="I32" t="s">
@@ -4472,7 +4475,7 @@
         <f t="shared" si="0"/>
         <v>201233</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33">
         <v>1645289</v>
       </c>
       <c r="I33" t="s">
@@ -4508,7 +4511,7 @@
         <f t="shared" si="0"/>
         <v>201238</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34">
         <v>1645290</v>
       </c>
       <c r="I34" t="s">
@@ -4544,7 +4547,7 @@
         <f t="shared" si="0"/>
         <v>201237</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35">
         <v>1645291</v>
       </c>
       <c r="I35" t="s">
@@ -4580,7 +4583,7 @@
         <f t="shared" si="0"/>
         <v>201236</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36">
         <v>1645292</v>
       </c>
       <c r="I36" t="s">
@@ -4616,7 +4619,7 @@
         <f t="shared" si="0"/>
         <v>201239</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37">
         <v>1645293</v>
       </c>
       <c r="I37" t="s">
@@ -4652,7 +4655,7 @@
         <f t="shared" si="0"/>
         <v>201240</v>
       </c>
-      <c r="H38" s="15">
+      <c r="H38">
         <v>1645294</v>
       </c>
       <c r="I38" t="s">
@@ -4688,7 +4691,7 @@
         <f t="shared" si="0"/>
         <v>201241</v>
       </c>
-      <c r="H39" s="15">
+      <c r="H39">
         <v>1645295</v>
       </c>
       <c r="I39" t="s">
@@ -4724,7 +4727,7 @@
         <f t="shared" si="0"/>
         <v>201244</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H40">
         <v>1645296</v>
       </c>
       <c r="I40" t="s">
@@ -4760,7 +4763,7 @@
         <f t="shared" si="0"/>
         <v>201243</v>
       </c>
-      <c r="H41" s="15">
+      <c r="H41">
         <v>1645297</v>
       </c>
       <c r="I41" t="s">
@@ -4796,7 +4799,7 @@
         <f t="shared" si="0"/>
         <v>201242</v>
       </c>
-      <c r="H42" s="15">
+      <c r="H42">
         <v>1645298</v>
       </c>
       <c r="I42" t="s">
@@ -4832,7 +4835,7 @@
         <f t="shared" si="0"/>
         <v>201247</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H43">
         <v>1645299</v>
       </c>
       <c r="I43" t="s">
@@ -5146,7 +5149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE4A661-52D8-45D9-824A-E6313569953C}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -5161,7 +5164,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2">
         <v>1645258</v>
       </c>
       <c r="B2" t="s">
@@ -5169,7 +5172,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+      <c r="A3">
         <v>1645259</v>
       </c>
       <c r="B3" t="s">
@@ -5177,7 +5180,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4">
         <v>1645260</v>
       </c>
       <c r="B4" t="s">
@@ -5185,7 +5188,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5">
         <v>1645261</v>
       </c>
       <c r="B5" t="s">
@@ -5193,7 +5196,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6">
         <v>1645262</v>
       </c>
       <c r="B6" t="s">
@@ -5201,7 +5204,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7">
         <v>1645263</v>
       </c>
       <c r="B7" t="s">
@@ -5209,7 +5212,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8">
         <v>1645264</v>
       </c>
       <c r="B8" t="s">
@@ -5217,7 +5220,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9">
         <v>1645265</v>
       </c>
       <c r="B9" t="s">
@@ -5225,7 +5228,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10">
         <v>1645266</v>
       </c>
       <c r="B10" t="s">
@@ -5233,7 +5236,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11">
         <v>1645267</v>
       </c>
       <c r="B11" t="s">
@@ -5241,7 +5244,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12">
         <v>1645268</v>
       </c>
       <c r="B12" t="s">
@@ -5249,7 +5252,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="A13">
         <v>1645269</v>
       </c>
       <c r="B13" t="s">
@@ -5257,7 +5260,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="A14">
         <v>1645270</v>
       </c>
       <c r="B14" t="s">
@@ -5265,7 +5268,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="A15">
         <v>1645271</v>
       </c>
       <c r="B15" t="s">
@@ -5273,7 +5276,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+      <c r="A16">
         <v>1645272</v>
       </c>
       <c r="B16" t="s">
@@ -5281,7 +5284,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="A17">
         <v>1645273</v>
       </c>
       <c r="B17" t="s">
@@ -5289,7 +5292,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+      <c r="A18">
         <v>1645274</v>
       </c>
       <c r="B18" t="s">
@@ -5297,7 +5300,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="A19">
         <v>1645275</v>
       </c>
       <c r="B19" t="s">
@@ -5305,7 +5308,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="A20">
         <v>1645276</v>
       </c>
       <c r="B20" t="s">
@@ -5313,7 +5316,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="A21">
         <v>1645277</v>
       </c>
       <c r="B21" t="s">
@@ -5321,7 +5324,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+      <c r="A22">
         <v>1645278</v>
       </c>
       <c r="B22" t="s">
@@ -5329,7 +5332,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="A23">
         <v>1645279</v>
       </c>
       <c r="B23" t="s">
@@ -5337,7 +5340,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="A24">
         <v>1645280</v>
       </c>
       <c r="B24" t="s">
@@ -5345,7 +5348,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="A25">
         <v>1645281</v>
       </c>
       <c r="B25" t="s">
@@ -5353,7 +5356,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="A26">
         <v>1645282</v>
       </c>
       <c r="B26" t="s">
@@ -5361,7 +5364,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+      <c r="A27">
         <v>1645283</v>
       </c>
       <c r="B27" t="s">
@@ -5369,7 +5372,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28">
         <v>1645284</v>
       </c>
       <c r="B28" t="s">
@@ -5377,7 +5380,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+      <c r="A29">
         <v>1645285</v>
       </c>
       <c r="B29" t="s">
@@ -5385,7 +5388,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+      <c r="A30">
         <v>1645286</v>
       </c>
       <c r="B30" t="s">
@@ -5393,7 +5396,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+      <c r="A31">
         <v>1645287</v>
       </c>
       <c r="B31" t="s">
@@ -5401,7 +5404,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+      <c r="A32">
         <v>1645288</v>
       </c>
       <c r="B32" t="s">
@@ -5409,7 +5412,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
+      <c r="A33">
         <v>1645289</v>
       </c>
       <c r="B33" t="s">
@@ -5417,7 +5420,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="A34">
         <v>1645290</v>
       </c>
       <c r="B34" t="s">
@@ -5425,7 +5428,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
+      <c r="A35">
         <v>1645291</v>
       </c>
       <c r="B35" t="s">
@@ -5433,7 +5436,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
+      <c r="A36">
         <v>1645292</v>
       </c>
       <c r="B36" t="s">
@@ -5441,7 +5444,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
+      <c r="A37">
         <v>1645293</v>
       </c>
       <c r="B37" t="s">
@@ -5449,7 +5452,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
+      <c r="A38">
         <v>1645294</v>
       </c>
       <c r="B38" t="s">
@@ -5457,7 +5460,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="15">
+      <c r="A39">
         <v>1645295</v>
       </c>
       <c r="B39" t="s">
@@ -5465,7 +5468,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
+      <c r="A40">
         <v>1645296</v>
       </c>
       <c r="B40" t="s">
@@ -5473,7 +5476,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
+      <c r="A41">
         <v>1645297</v>
       </c>
       <c r="B41" t="s">
@@ -5481,7 +5484,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
+      <c r="A42">
         <v>1645298</v>
       </c>
       <c r="B42" t="s">
@@ -5489,7 +5492,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
+      <c r="A43">
         <v>1645299</v>
       </c>
       <c r="B43" t="s">
@@ -8606,8 +8609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DEAEC3-E597-43CF-8A39-542D98AFB6F7}">
   <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9227,7 +9230,7 @@
         <v>140</v>
       </c>
       <c r="C12">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>201251</v>
@@ -9255,7 +9258,7 @@
       </c>
       <c r="N12" t="str">
         <f>IF(C12="", "", _xlfn.XLOOKUP(C12, Sheet1!A:A, Sheet1!B:B, ""))</f>
-        <v>3DD.003E185F84</v>
+        <v>3DD.003E185F67</v>
       </c>
       <c r="O12" t="str">
         <f>IF(D12="", "", _xlfn.XLOOKUP(D12, Sheet1!F:F, Sheet1!E:E, ""))</f>
@@ -9647,7 +9650,6 @@
       <c r="F38" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="Q2:Q100">
     <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>AND($Q2&lt;&gt;$B2, $Q2&lt;&gt;"UKN", $Q2&lt;&gt;"", $B2&lt;&gt;"")</formula>

</xml_diff>